<commit_message>
updated python marketing project with jupyter notebook and PCA
</commit_message>
<xml_diff>
--- a/Python/ML-Marketing/confusion, classification reports.xlsx
+++ b/Python/ML-Marketing/confusion, classification reports.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="1380" windowWidth="28860" windowHeight="19080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6740" yWindow="1160" windowWidth="28860" windowHeight="19080" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Deposit correlation matrix" sheetId="2" r:id="rId2"/>
+    <sheet name="Deposit correlation matrix" sheetId="2" r:id="rId1"/>
+    <sheet name="Confusionmatrix" sheetId="1" r:id="rId2"/>
+    <sheet name="Metrics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="83">
   <si>
     <t>KNN confusion matrix</t>
   </si>
@@ -170,13 +171,114 @@
   </si>
   <si>
     <t>Correlation to Deposit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deposit
+Correlation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y  </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Percentage of succesfull term deposits based on poutcome_success</t>
+  </si>
+  <si>
+    <t>term deposit w/  poutcome success</t>
+  </si>
+  <si>
+    <t>term deposits w/ no poutcome
+success</t>
+  </si>
+  <si>
+    <t>total poutcome_success</t>
+  </si>
+  <si>
+    <t>term deposit w/ poutcome success</t>
+  </si>
+  <si>
+    <t>avg / total</t>
+  </si>
+  <si>
+    <t>Term Deposit</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Parameters tuned</t>
+  </si>
+  <si>
+    <t>Parameters used</t>
+  </si>
+  <si>
+    <t>Best parameters</t>
+  </si>
+  <si>
+    <t>Avg cross val score</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_neighbors </t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>n_estimators</t>
+  </si>
+  <si>
+    <t>criterion</t>
+  </si>
+  <si>
+    <t>'gini,'entropy'</t>
+  </si>
+  <si>
+    <t>2 to 22</t>
+  </si>
+  <si>
+    <t>gini</t>
+  </si>
+  <si>
+    <t>5 to 25</t>
+  </si>
+  <si>
+    <t>n = 18</t>
+  </si>
+  <si>
+    <t>SVC</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>kernel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 to 1.5 </t>
+  </si>
+  <si>
+    <t>linear', 'rbf'</t>
+  </si>
+  <si>
+    <t>rbf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -207,6 +309,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -234,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -285,8 +414,344 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -333,8 +798,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -357,8 +884,161 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="18" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="19" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="2" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="26" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="27" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -381,6 +1061,37 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -403,6 +1114,37 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="41" builtinId="5"/>
   </cellStyles>
@@ -733,9 +1475,369 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.30678800000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.30678800000000001</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.13587299999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0.13587299999999999</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.103621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0.103621</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.102895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.102895</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="13">
+        <v>9.3235999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="13">
+        <v>9.3235999999999999E-2</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="13">
+        <v>6.6447999999999993E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="13">
+        <v>6.6447999999999993E-2</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="13">
+        <v>-7.2082999999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="13">
+        <v>6.3525999999999999E-2</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="13">
+        <v>-7.3172000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="13">
+        <v>5.2838000000000003E-2</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="13">
+        <v>-0.13917299999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="13">
+        <v>3.2453999999999997E-2</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="13">
+        <v>-0.15093500000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2.5155E-2</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="13">
+        <v>-0.16686300000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="13">
+        <v>1.8717000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1.4042000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="13">
+        <v>1.2052999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="13">
+        <v>9.8849999999999997E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="13">
+        <v>2.7720000000000002E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="13">
+        <v>8.5499999999999997E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="13">
+        <v>-8.9700000000000005E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="13">
+        <v>-1.9661999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="13">
+        <v>-2.2419000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="13">
+        <v>-2.8348000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="13">
+        <v>-3.2486000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="13">
+        <v>-3.6387999999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="13">
+        <v>-4.0392999999999998E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="13">
+        <v>-6.0260000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="13">
+        <v>-6.8184999999999996E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="13">
+        <v>-7.2082999999999994E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="13">
+        <v>-7.3172000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="13">
+        <v>-0.13917299999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="13">
+        <v>-0.15093500000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="13">
+        <v>-0.16686300000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -1092,282 +2194,337 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A2:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="28" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13">
+    <row r="2" spans="1:17">
+      <c r="A2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="15">
+        <v>39389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="49"/>
+      <c r="B4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="16">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="16">
+        <v>4311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="16" thickBot="1">
+      <c r="A6" s="49"/>
+      <c r="B6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="17">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="16" thickTop="1">
+      <c r="A7" s="21"/>
+      <c r="B7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="24">
+        <f>SUM(C3:C6)</f>
+        <v>45211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="16" thickBot="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:17" ht="34" customHeight="1" thickBot="1">
+      <c r="A9" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="15">
+        <f>C6</f>
+        <v>978</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17" customHeight="1" thickBot="1">
+      <c r="A10" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="15">
+        <f>SUM(C4,C6)</f>
+        <v>1511</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="39">
+        <v>0.88919999999999999</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="O10" s="42">
+        <v>0.99</v>
+      </c>
+      <c r="P10" s="42">
+        <v>0.94</v>
+      </c>
+      <c r="Q10" s="41">
+        <v>7986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="18" customHeight="1" thickBot="1">
+      <c r="A11" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="53"/>
+      <c r="C11" s="55">
+        <f>C9/C10</f>
+        <v>0.64725347452018533</v>
+      </c>
+      <c r="G11" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="35">
+        <v>20</v>
+      </c>
+      <c r="K11" s="54">
+        <v>0.88549999999999995</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="47">
+        <v>0.61</v>
+      </c>
+      <c r="O11" s="47">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P11" s="47">
+        <v>0.23</v>
+      </c>
+      <c r="Q11" s="48">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="16" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="55"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="63"/>
+      <c r="M12" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="44">
+        <v>0.86</v>
+      </c>
+      <c r="O12" s="44">
+        <v>0.89</v>
+      </c>
+      <c r="P12" s="44">
+        <v>0.86</v>
+      </c>
+      <c r="Q12" s="45">
+        <v>9043</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="21" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="G13" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="13">
-        <v>0.30678800000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="13">
-        <v>0.13587299999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="13">
-        <v>0.103621</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="13">
-        <v>0.102895</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="13">
-        <v>9.3235999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="13">
-        <v>6.6447999999999993E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="13">
-        <v>6.3525999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="13">
-        <v>5.2838000000000003E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="13">
-        <v>3.2453999999999997E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="13">
-        <v>2.5155E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="13">
-        <v>1.8717000000000001E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="13">
-        <v>1.4042000000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="13">
-        <v>1.2052999999999999E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="13">
-        <v>9.8849999999999997E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="13">
-        <v>2.7720000000000002E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="13">
-        <v>8.5499999999999997E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="13">
-        <v>-8.9700000000000005E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="13">
-        <v>-1.9661999999999999E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="13">
-        <v>-2.2419000000000001E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="13">
-        <v>-2.8348000000000002E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="13">
-        <v>-3.2486000000000001E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="13">
-        <v>-3.6387999999999997E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="13">
-        <v>-4.0392999999999998E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="13">
-        <v>-6.0260000000000001E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="13">
-        <v>-6.8184999999999996E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="13">
-        <v>-7.2082999999999994E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="13">
-        <v>-7.3172000000000001E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="13">
-        <v>-0.13917299999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="13">
-        <v>-0.15093500000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="13">
-        <v>-0.16686300000000001</v>
-      </c>
+      <c r="K13" s="65">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="22" customHeight="1" thickBot="1">
+      <c r="A14" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="51"/>
+      <c r="C14" s="15">
+        <v>978</v>
+      </c>
+      <c r="G14" s="59"/>
+      <c r="H14" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="66"/>
+      <c r="M14" s="40"/>
+    </row>
+    <row r="15" spans="1:17" ht="33" customHeight="1" thickBot="1">
+      <c r="A15" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="22">
+        <v>4311</v>
+      </c>
+      <c r="M15" s="40"/>
+    </row>
+    <row r="16" spans="1:17" ht="33" customHeight="1" thickTop="1">
+      <c r="A16" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="23">
+        <f>SUM(C14:C15)</f>
+        <v>5289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="53"/>
+      <c r="C17" s="55">
+        <f>C14/C16</f>
+        <v>0.18491208167895631</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="31" customHeight="1">
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="55"/>
     </row>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B12"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>